<commit_message>
Implement four quarters in hour
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/02-many-tasks/02-many-tasks.xlsx
+++ b/ampl-data-input-excel/02-many-tasks/02-many-tasks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="61">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -315,7 +315,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -378,10 +378,6 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -570,7 +566,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -646,7 +642,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -671,29 +667,74 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
@@ -765,7 +806,7 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -773,7 +814,7 @@
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="19.48"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="3" style="16" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="3" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2112,8 +2153,8 @@
   </sheetPr>
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3219,7 +3260,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>